<commit_message>
1. soru analitik doğrulanmaya çalışıldı
bu noktada maxwell üzerinden istenen inductance değeri elde edilemedi, denenen yöntemlerin hiçbiri işe yaramadı
</commit_message>
<xml_diff>
--- a/Project1/p1_question2.xlsx
+++ b/Project1/p1_question2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="79">
   <si>
     <t>Iin</t>
   </si>
@@ -201,9 +201,6 @@
     <t>Total Copper loss(W)</t>
   </si>
   <si>
-    <t>lamination</t>
-  </si>
-  <si>
     <t>B-H curve kullanılarak yazılır</t>
   </si>
   <si>
@@ -241,6 +238,21 @@
   </si>
   <si>
     <t>aşağıda görsel boyutları göstermek içindir.</t>
+  </si>
+  <si>
+    <t>lamination type</t>
+  </si>
+  <si>
+    <t>no lamination</t>
+  </si>
+  <si>
+    <t>material cost ($/kg)</t>
+  </si>
+  <si>
+    <t>cable cost($/m)</t>
+  </si>
+  <si>
+    <t>outer inductance,L2(H)</t>
   </si>
 </sst>
 </file>
@@ -421,7 +433,7 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -437,7 +449,6 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="2" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="2" applyFill="1"/>
@@ -864,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="L40" sqref="L40"/>
+    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -885,7 +896,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="7" t="s">
         <v>26</v>
       </c>
     </row>
@@ -900,11 +911,11 @@
         <v>2</v>
       </c>
       <c r="C4" s="3"/>
-      <c r="F4" s="8" t="s">
+      <c r="F4" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="8" t="s">
-        <v>73</v>
+      <c r="G4" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="K4" s="3" t="s">
         <v>14</v>
@@ -912,215 +923,212 @@
       <c r="L4" s="3"/>
     </row>
     <row r="5" spans="2:14">
-      <c r="B5" s="8" t="s">
+      <c r="B5" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="18">
+      <c r="C5" s="17">
         <v>500000</v>
       </c>
-      <c r="F5" t="s">
-        <v>61</v>
-      </c>
-      <c r="K5" s="8" t="s">
+      <c r="F5" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="G5" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="K5" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="L5" s="14">
+      <c r="L5" s="13">
         <v>350</v>
       </c>
     </row>
     <row r="6" spans="2:14">
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="18">
+      <c r="C6" s="17">
         <v>34500</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="10" t="s">
+      <c r="K6" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="L6" s="13">
+      <c r="L6" s="12">
         <f>L5/L9</f>
         <v>253.62318840579712</v>
       </c>
     </row>
     <row r="7" spans="2:14">
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="18">
+      <c r="C7" s="17">
         <v>25000</v>
       </c>
-      <c r="F7" s="8" t="s">
+      <c r="F7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="18">
+      <c r="G7" s="17">
         <v>1.2</v>
       </c>
-      <c r="H7" s="26" t="s">
+      <c r="H7" s="25" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="2:14">
+      <c r="B8" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="17">
+        <v>50</v>
+      </c>
+      <c r="F8" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="G8" s="17">
+        <v>1000</v>
+      </c>
+      <c r="H8" s="25"/>
+    </row>
+    <row r="9" spans="2:14" ht="24.75">
+      <c r="B9" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="C9" s="17">
+        <v>40</v>
+      </c>
+      <c r="F9" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="G9" s="17">
+        <v>0.95</v>
+      </c>
+      <c r="H9" s="23" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="8" spans="2:14">
-      <c r="B8" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="18">
-        <v>50</v>
-      </c>
-      <c r="F8" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="G8" s="18">
-        <v>1000</v>
-      </c>
-      <c r="H8" s="26"/>
-    </row>
-    <row r="9" spans="2:14" ht="24.75">
-      <c r="B9" s="8" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="18">
-        <v>40</v>
-      </c>
-      <c r="F9" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="G9" s="18">
-        <v>0.95</v>
-      </c>
-      <c r="H9" s="24" t="s">
-        <v>63</v>
-      </c>
-      <c r="K9" s="10" t="s">
+      <c r="K9" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="11">
+      <c r="L9" s="10">
         <f>C6/C7</f>
         <v>1.38</v>
       </c>
     </row>
     <row r="10" spans="2:14">
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="7" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="18">
+      <c r="C10" s="17">
         <v>3</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="22">
+      <c r="G10" s="21">
         <v>7.85</v>
       </c>
     </row>
     <row r="11" spans="2:14">
-      <c r="B11" s="8" t="s">
+      <c r="B11" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="18">
+      <c r="C11" s="17">
         <v>0.3</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="F11" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="G11" s="7"/>
+    </row>
+    <row r="12" spans="2:14">
+      <c r="B12" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="C12" s="17">
+        <v>1</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="G11" s="3"/>
-    </row>
-    <row r="12" spans="2:14">
-      <c r="B12" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" s="18">
-        <v>1</v>
-      </c>
-      <c r="F12" s="8" t="s">
+      <c r="G12" s="3"/>
+    </row>
+    <row r="13" spans="2:14">
+      <c r="F13" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G13" s="7" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="13" spans="2:14">
-      <c r="F13" s="8" t="s">
-        <v>44</v>
-      </c>
-      <c r="G13" s="18">
-        <v>1.6800000000000002E-8</v>
-      </c>
-      <c r="L13" s="17" t="s">
+      <c r="L13" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="M13" s="17" t="s">
+      <c r="M13" s="16" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="2:14">
-      <c r="B14" s="10" t="s">
+      <c r="B14" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="11">
+      <c r="C14" s="10">
         <f>C5/C6</f>
         <v>14.492753623188406</v>
       </c>
-      <c r="K14" s="10" t="s">
+      <c r="F14" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="G14" s="17">
+        <v>1.6800000000000002E-8</v>
+      </c>
+      <c r="K14" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="L14" s="10">
+      <c r="L14" s="9">
         <f>M14/10^6</f>
         <v>1.1272141706924315E-2</v>
       </c>
-      <c r="M14" s="10">
+      <c r="M14" s="9">
         <f>(L5*C19+L6*C20)/C11</f>
         <v>11272.141706924316</v>
       </c>
     </row>
     <row r="15" spans="2:14">
-      <c r="B15" s="10" t="s">
+      <c r="B15" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="11">
+      <c r="C15" s="10">
         <f>C5/C7</f>
         <v>20</v>
       </c>
+      <c r="F15" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="G15" s="7"/>
     </row>
     <row r="16" spans="2:14">
-      <c r="F16" s="10" t="s">
-        <v>64</v>
-      </c>
-      <c r="G16" s="19">
-        <f>G7/G8</f>
-        <v>1.1999999999999999E-3</v>
-      </c>
-      <c r="H16" s="1"/>
       <c r="K16" s="5" t="s">
-        <v>70</v>
-      </c>
-      <c r="L16" s="10">
+        <v>69</v>
+      </c>
+      <c r="L16" s="9">
         <f>SQRT(L14)</f>
         <v>0.10617034287843435</v>
       </c>
-      <c r="M16" s="10">
+      <c r="M16" s="9">
         <f>SQRT(M14)</f>
         <v>106.17034287843435</v>
       </c>
-      <c r="N16" s="25" t="s">
-        <v>68</v>
+      <c r="N16" s="24" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="2:14">
-      <c r="F17" s="10" t="s">
-        <v>65</v>
-      </c>
-      <c r="G17" s="19">
-        <f>G7/G8/4/3.14*10^7</f>
-        <v>955.41401273885333</v>
-      </c>
-      <c r="N17" s="25"/>
+      <c r="H17" s="1"/>
+      <c r="N17" s="24"/>
     </row>
     <row r="18" spans="2:14">
       <c r="C18" s="6" t="s">
@@ -1129,55 +1137,63 @@
       <c r="D18" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="N18" s="25"/>
+      <c r="F18" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="G18" s="18">
+        <f>G7/G8</f>
+        <v>1.1999999999999999E-3</v>
+      </c>
+      <c r="N18" s="24"/>
     </row>
     <row r="19" spans="2:14">
-      <c r="B19" s="10" t="s">
+      <c r="B19" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="10">
+      <c r="C19" s="9">
         <f>C14/C10</f>
         <v>4.8309178743961354</v>
       </c>
-      <c r="D19" s="10">
+      <c r="D19" s="9">
         <f>C19/1000000</f>
         <v>4.8309178743961353E-6</v>
       </c>
-      <c r="K19" s="15" t="s">
+      <c r="F19" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="G19" s="18">
+        <f>G7/G8/4/3.14*10^7</f>
+        <v>955.41401273885333</v>
+      </c>
+      <c r="K19" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="L19" s="16" t="s">
+      <c r="L19" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="M19" s="16" t="s">
+      <c r="M19" s="15" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="20" spans="2:14">
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="9">
         <f>C15/C10</f>
         <v>6.666666666666667</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="9">
         <f>C20/1000000</f>
         <v>6.6666666666666666E-6</v>
       </c>
-      <c r="G20" s="16" t="s">
-        <v>17</v>
-      </c>
-      <c r="H20" s="16" t="s">
-        <v>18</v>
-      </c>
-      <c r="K20" s="8" t="s">
+      <c r="K20" s="7" t="s">
         <v>41</v>
       </c>
-      <c r="L20" s="8">
+      <c r="L20" s="7">
         <v>0.106</v>
       </c>
-      <c r="M20" s="8">
+      <c r="M20" s="7">
         <f>L20*1000</f>
         <v>106</v>
       </c>
@@ -1186,16 +1202,11 @@
       </c>
     </row>
     <row r="21" spans="2:14">
-      <c r="F21" s="10" t="s">
-        <v>32</v>
-      </c>
-      <c r="G21" s="11">
-        <f>C6/4.44/L5/C8/G7</f>
-        <v>0.37001287001287003</v>
-      </c>
-      <c r="H21" s="10">
-        <f>1000000*G21</f>
-        <v>370012.87001287006</v>
+      <c r="G21" s="15" t="s">
+        <v>17</v>
+      </c>
+      <c r="H21" s="15" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="2:14">
@@ -1205,125 +1216,125 @@
       <c r="D22" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="K22" s="10" t="s">
+      <c r="F22" s="9" t="s">
+        <v>32</v>
+      </c>
+      <c r="G22" s="10">
+        <f>C6/4.44/L5/C8/G7</f>
+        <v>0.37001287001287003</v>
+      </c>
+      <c r="H22" s="9">
+        <f>1000000*G22</f>
+        <v>370012.87001287006</v>
+      </c>
+      <c r="K22" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="L22" s="10">
+      <c r="L22" s="9">
         <f>L14/L20</f>
         <v>0.106340959499286</v>
       </c>
-      <c r="M22" s="10">
+      <c r="M22" s="9">
         <f>M14/M20</f>
         <v>106.340959499286</v>
       </c>
     </row>
     <row r="23" spans="2:14">
-      <c r="B23" s="10" t="s">
+      <c r="B23" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="9">
+      <c r="C23" s="8">
         <v>1.24</v>
       </c>
       <c r="D23" s="5">
         <f>SQRT(C19/3.14)</f>
         <v>1.2403664285993157</v>
       </c>
-      <c r="G23" s="16" t="s">
-        <v>20</v>
-      </c>
-      <c r="H23" s="16" t="s">
-        <v>21</v>
-      </c>
       <c r="K23" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="24" spans="2:14">
-      <c r="B24" s="10" t="s">
+    <row r="24" spans="2:14" ht="15" customHeight="1">
+      <c r="B24" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="9">
+      <c r="C24" s="8">
         <v>1.4570000000000001</v>
       </c>
       <c r="D24" s="5">
         <f>SQRT(C20/3.14)</f>
         <v>1.4571006315731201</v>
       </c>
-      <c r="F24" s="10" t="s">
+      <c r="G24" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="H24" s="15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="25" spans="2:14" ht="15" customHeight="1">
+      <c r="B25" s="24" t="s">
+        <v>68</v>
+      </c>
+      <c r="C25" s="24"/>
+      <c r="D25" s="24"/>
+      <c r="F25" s="9" t="s">
+        <v>66</v>
+      </c>
+      <c r="G25" s="9">
+        <f>SQRT(G22)</f>
+        <v>0.60828683202324052</v>
+      </c>
+      <c r="H25" s="9">
+        <f>SQRT(H22)</f>
+        <v>608.28683202324055</v>
+      </c>
+      <c r="I25" s="24" t="s">
         <v>67</v>
       </c>
-      <c r="G24" s="10">
-        <f>SQRT(G21)</f>
-        <v>0.60828683202324052</v>
-      </c>
-      <c r="H24" s="10">
-        <f>SQRT(H21)</f>
-        <v>608.28683202324055</v>
-      </c>
-      <c r="I24" s="25" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="25" spans="2:14" ht="15" customHeight="1">
-      <c r="B25" s="25" t="s">
-        <v>69</v>
-      </c>
-      <c r="C25" s="25"/>
-      <c r="D25" s="25"/>
-      <c r="I25" s="25"/>
     </row>
     <row r="26" spans="2:14">
-      <c r="B26" s="25"/>
-      <c r="C26" s="25"/>
-      <c r="D26" s="25"/>
-      <c r="F26" s="15" t="s">
+      <c r="B26" s="24"/>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="I26" s="24"/>
+    </row>
+    <row r="27" spans="2:14">
+      <c r="B27" s="24"/>
+      <c r="C27" s="24"/>
+      <c r="D27" s="24"/>
+      <c r="F27" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="G26" s="16" t="s">
+      <c r="G27" s="15" t="s">
         <v>20</v>
       </c>
-      <c r="H26" s="16" t="s">
+      <c r="H27" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="I26" s="25"/>
-    </row>
-    <row r="27" spans="2:14">
-      <c r="B27" s="25"/>
-      <c r="C27" s="25"/>
-      <c r="D27" s="25"/>
-      <c r="F27" s="8" t="s">
+      <c r="I27" s="24"/>
+    </row>
+    <row r="28" spans="2:14">
+      <c r="F28" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G27" s="8">
+      <c r="G28" s="7">
         <v>0.60799999999999998</v>
       </c>
-      <c r="H27" s="8">
-        <f>G27*1000</f>
+      <c r="H28" s="7">
+        <f>G28*1000</f>
         <v>608</v>
       </c>
-    </row>
-    <row r="28" spans="2:14">
-      <c r="L28" s="16" t="s">
+      <c r="L28" s="15" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="29" spans="2:14">
-      <c r="F29" s="10" t="s">
-        <v>52</v>
-      </c>
-      <c r="G29" s="10">
-        <f>G21/G27</f>
-        <v>0.60857379936327305</v>
-      </c>
-      <c r="H29" s="10">
-        <f>H21/H27</f>
-        <v>608.57379936327311</v>
-      </c>
-      <c r="K29" s="10" t="s">
+      <c r="K29" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="L29" s="10">
-        <f>L20+2*G29</f>
+      <c r="L29" s="9">
+        <f>L20+2*G30</f>
         <v>1.3231475987265462</v>
       </c>
     </row>
@@ -1331,29 +1342,40 @@
       <c r="C30" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="F30" t="s">
+      <c r="F30" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="G30" s="9">
+        <f>G22/G28</f>
+        <v>0.60857379936327305</v>
+      </c>
+      <c r="H30" s="9">
+        <f>H22/H28</f>
+        <v>608.57379936327311</v>
+      </c>
+      <c r="K30" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="L30" s="9">
+        <f>L22+2*G30</f>
+        <v>1.323488558225832</v>
+      </c>
+    </row>
+    <row r="31" spans="2:14">
+      <c r="B31" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="9">
+        <f>SQRT(H28*H30)/2 + M22/4</f>
+        <v>330.7286558864418</v>
+      </c>
+      <c r="F31" t="s">
         <v>38</v>
       </c>
-      <c r="K30" s="10" t="s">
-        <v>53</v>
-      </c>
-      <c r="L30" s="10">
-        <f>L22+2*G29</f>
-        <v>1.323488558225832</v>
-      </c>
-    </row>
-    <row r="31" spans="2:14">
-      <c r="B31" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="C31" s="10">
-        <f>SQRT(H27*H29)/2 + M22/4</f>
-        <v>330.7286558864418</v>
-      </c>
-      <c r="K31" s="23" t="s">
+      <c r="K31" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="L31" s="23"/>
+      <c r="L31" s="22"/>
     </row>
     <row r="33" spans="2:12">
       <c r="C33" s="6" t="s">
@@ -1362,125 +1384,132 @@
       <c r="D33" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="G33" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="H33" s="17" t="s">
-        <v>56</v>
-      </c>
     </row>
     <row r="34" spans="2:12">
-      <c r="B34" s="10" t="s">
+      <c r="B34" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="10">
+      <c r="C34" s="9">
         <f>2*3.14*C31*L5</f>
         <v>726941.58563839912</v>
       </c>
-      <c r="D34" s="10">
+      <c r="D34" s="9">
         <f>C34/1000</f>
         <v>726.94158563839915</v>
       </c>
-      <c r="F34" s="10" t="s">
-        <v>50</v>
-      </c>
-      <c r="G34" s="10">
-        <f>(L29*L30-L20*L22)*G27*1000000*G10</f>
-        <v>8304187.8760512844</v>
-      </c>
-      <c r="H34" s="10">
-        <f>G34/1000</f>
-        <v>8304.1878760512845</v>
+      <c r="G34" s="16" t="s">
+        <v>55</v>
+      </c>
+      <c r="H34" s="16" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="35" spans="2:12">
-      <c r="B35" s="10" t="s">
+      <c r="B35" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="10">
+      <c r="C35" s="9">
         <f>2*3.14*C31*L6</f>
         <v>526769.26495536172</v>
       </c>
-      <c r="D35" s="10">
+      <c r="D35" s="9">
         <f>C35/1000</f>
         <v>526.76926495536168</v>
       </c>
-      <c r="L35" s="16" t="s">
+      <c r="F35" s="9" t="s">
+        <v>50</v>
+      </c>
+      <c r="G35" s="9">
+        <f>(L29*L30-L20*L22)*G28*1000000*G10</f>
+        <v>8304187.8760512844</v>
+      </c>
+      <c r="H35" s="9">
+        <f>G35/1000</f>
+        <v>8304.1878760512845</v>
+      </c>
+      <c r="L35" s="15" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="36" spans="2:12">
-      <c r="K36" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="L36" s="7">
-        <f>2*L20+2*L22+4*G29</f>
+      <c r="K36" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="L36" s="9">
+        <f>2*L20+2*L22+4*G30</f>
         <v>2.8589771164516642</v>
       </c>
     </row>
     <row r="39" spans="2:12">
-      <c r="B39" s="10" t="s">
+      <c r="B39" s="9" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="10">
-        <f>G13*D34/D19</f>
+      <c r="C39" s="9">
+        <f>G14*D34/D19</f>
         <v>2.5280120582160972</v>
       </c>
     </row>
     <row r="40" spans="2:12">
-      <c r="B40" s="10" t="s">
+      <c r="B40" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="C40" s="10">
-        <f>G13*D35/3.14/(C24*0.001)^2</f>
+      <c r="C40" s="9">
+        <f>G14*D35/3.14/(C24*0.001)^2</f>
         <v>1.3276419229175465</v>
       </c>
-      <c r="K40" t="s">
-        <v>71</v>
-      </c>
-      <c r="L40">
-        <f>L36/G21/G16</f>
+      <c r="K40" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="L40" s="9">
+        <f>L36/G22/G18</f>
         <v>6438.9136796607045</v>
       </c>
     </row>
     <row r="42" spans="2:12">
-      <c r="B42" s="20" t="s">
+      <c r="B42" s="19" t="s">
         <v>46</v>
       </c>
-      <c r="C42" s="21">
+      <c r="C42" s="20">
         <f>(C14^2)*C39</f>
         <v>530.98341907500469</v>
       </c>
-      <c r="K42" t="s">
-        <v>72</v>
-      </c>
-      <c r="L42">
+      <c r="K42" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="L42" s="9">
         <f>(L5^2)/L40</f>
         <v>19.024948321166978</v>
       </c>
     </row>
     <row r="43" spans="2:12">
-      <c r="B43" s="20" t="s">
+      <c r="B43" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="C43" s="21">
+      <c r="C43" s="20">
         <f>(C15^2)*C40</f>
         <v>531.05676916701862</v>
       </c>
+      <c r="K43" s="9" t="s">
+        <v>78</v>
+      </c>
+      <c r="L43" s="9">
+        <f>L6^2/L40</f>
+        <v>9.9899959678465553</v>
+      </c>
     </row>
     <row r="44" spans="2:12">
-      <c r="B44" s="20" t="s">
+      <c r="B44" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="21">
+      <c r="C44" s="20">
         <f>C42+C43</f>
         <v>1062.0401882420233</v>
       </c>
-      <c r="F44" s="20" t="s">
+      <c r="F44" s="19" t="s">
         <v>57</v>
       </c>
-      <c r="G44" s="20">
-        <f>G9*(G7^2)*H34</f>
+      <c r="G44" s="19">
+        <f>G9*(G7^2)*H35</f>
         <v>11360.129014438156</v>
       </c>
     </row>
@@ -1495,7 +1524,7 @@
     </row>
     <row r="51" spans="8:10">
       <c r="H51" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="I51" s="2"/>
       <c r="J51" s="2"/>
@@ -1509,13 +1538,13 @@
   <mergeCells count="10">
     <mergeCell ref="K31:L31"/>
     <mergeCell ref="H7:H8"/>
-    <mergeCell ref="I24:I26"/>
     <mergeCell ref="N16:N18"/>
     <mergeCell ref="H51:J52"/>
+    <mergeCell ref="I25:I27"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="K4:L4"/>
-    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="F12:G12"/>
     <mergeCell ref="B25:D27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
problem 1, 5. kısım dısında matlabda yapıldı
</commit_message>
<xml_diff>
--- a/Project1/p1_question2.xlsx
+++ b/Project1/p1_question2.xlsx
@@ -438,12 +438,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -466,17 +460,23 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="2" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="11" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -875,8 +875,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:N52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B10" workbookViewId="0">
-      <selection activeCell="J30" sqref="J30"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -896,357 +896,357 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="5" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="2:14">
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="25" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="3"/>
+      <c r="G3" s="25"/>
     </row>
     <row r="4" spans="2:14">
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="F4" s="7" t="s">
+      <c r="C4" s="25"/>
+      <c r="F4" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="7" t="s">
+      <c r="G4" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="K4" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="3"/>
+      <c r="L4" s="25"/>
     </row>
     <row r="5" spans="2:14">
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="17">
+      <c r="C5" s="15">
         <v>500000</v>
       </c>
-      <c r="F5" s="7" t="s">
+      <c r="F5" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="G5" s="7" t="s">
+      <c r="G5" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="K5" s="7" t="s">
+      <c r="K5" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="L5" s="13">
+      <c r="L5" s="11">
         <v>350</v>
       </c>
     </row>
     <row r="6" spans="2:14">
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="15">
         <v>34500</v>
       </c>
-      <c r="F6" s="7" t="s">
+      <c r="F6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="7" t="s">
+      <c r="G6" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="9" t="s">
+      <c r="K6" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="L6" s="12">
+      <c r="L6" s="10">
         <f>L5/L9</f>
         <v>253.62318840579712</v>
       </c>
     </row>
     <row r="7" spans="2:14">
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="15">
         <v>25000</v>
       </c>
-      <c r="F7" s="7" t="s">
+      <c r="F7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="17">
+      <c r="G7" s="15">
         <v>1.2</v>
       </c>
-      <c r="H7" s="25" t="s">
+      <c r="H7" s="22" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="8" spans="2:14">
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="15">
         <v>50</v>
       </c>
-      <c r="F8" s="7" t="s">
+      <c r="F8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="17">
+      <c r="G8" s="15">
         <v>1000</v>
       </c>
-      <c r="H8" s="25"/>
+      <c r="H8" s="22"/>
     </row>
     <row r="9" spans="2:14" ht="24.75">
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="15">
         <v>40</v>
       </c>
-      <c r="F9" s="7" t="s">
+      <c r="F9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="17">
+      <c r="G9" s="15">
         <v>0.95</v>
       </c>
-      <c r="H9" s="23" t="s">
+      <c r="H9" s="20" t="s">
         <v>62</v>
       </c>
-      <c r="K9" s="9" t="s">
+      <c r="K9" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="10">
+      <c r="L9" s="8">
         <f>C6/C7</f>
         <v>1.38</v>
       </c>
     </row>
     <row r="10" spans="2:14">
-      <c r="B10" s="7" t="s">
+      <c r="B10" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="15">
         <v>3</v>
       </c>
-      <c r="F10" s="11" t="s">
+      <c r="F10" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="21">
+      <c r="G10" s="19">
         <v>7.85</v>
       </c>
     </row>
     <row r="11" spans="2:14">
-      <c r="B11" s="7" t="s">
+      <c r="B11" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="15">
         <v>0.3</v>
       </c>
-      <c r="F11" s="7" t="s">
+      <c r="F11" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="G11" s="7"/>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" spans="2:14">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="15">
         <v>1</v>
       </c>
-      <c r="F12" s="3" t="s">
+      <c r="F12" s="25" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="3"/>
+      <c r="G12" s="25"/>
     </row>
     <row r="13" spans="2:14">
-      <c r="F13" s="7" t="s">
+      <c r="F13" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="7" t="s">
+      <c r="G13" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="L13" s="16" t="s">
+      <c r="L13" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="M13" s="16" t="s">
+      <c r="M13" s="14" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="2:14">
-      <c r="B14" s="9" t="s">
+      <c r="B14" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="10">
+      <c r="C14" s="8">
         <f>C5/C6</f>
         <v>14.492753623188406</v>
       </c>
-      <c r="F14" s="7" t="s">
+      <c r="F14" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="17">
+      <c r="G14" s="15">
         <v>1.6800000000000002E-8</v>
       </c>
-      <c r="K14" s="9" t="s">
+      <c r="K14" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="L14" s="9">
+      <c r="L14" s="7">
         <f>M14/10^6</f>
         <v>1.1272141706924315E-2</v>
       </c>
-      <c r="M14" s="9">
+      <c r="M14" s="7">
         <f>(L5*C19+L6*C20)/C11</f>
         <v>11272.141706924316</v>
       </c>
     </row>
     <row r="15" spans="2:14">
-      <c r="B15" s="9" t="s">
+      <c r="B15" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="10">
+      <c r="C15" s="8">
         <f>C5/C7</f>
         <v>20</v>
       </c>
-      <c r="F15" s="7" t="s">
+      <c r="F15" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="G15" s="7"/>
+      <c r="G15" s="5"/>
     </row>
     <row r="16" spans="2:14">
-      <c r="K16" s="5" t="s">
+      <c r="K16" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="L16" s="9">
+      <c r="L16" s="7">
         <f>SQRT(L14)</f>
         <v>0.10617034287843435</v>
       </c>
-      <c r="M16" s="9">
+      <c r="M16" s="7">
         <f>SQRT(M14)</f>
         <v>106.17034287843435</v>
       </c>
-      <c r="N16" s="24" t="s">
+      <c r="N16" s="23" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="17" spans="2:14">
       <c r="H17" s="1"/>
-      <c r="N17" s="24"/>
+      <c r="N17" s="23"/>
     </row>
     <row r="18" spans="2:14">
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="9" t="s">
+      <c r="F18" s="7" t="s">
         <v>63</v>
       </c>
-      <c r="G18" s="18">
+      <c r="G18" s="16">
         <f>G7/G8</f>
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="N18" s="24"/>
+      <c r="N18" s="23"/>
     </row>
     <row r="19" spans="2:14">
-      <c r="B19" s="9" t="s">
+      <c r="B19" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="9">
+      <c r="C19" s="7">
         <f>C14/C10</f>
         <v>4.8309178743961354</v>
       </c>
-      <c r="D19" s="9">
+      <c r="D19" s="7">
         <f>C19/1000000</f>
         <v>4.8309178743961353E-6</v>
       </c>
-      <c r="F19" s="9" t="s">
+      <c r="F19" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="G19" s="18">
+      <c r="G19" s="16">
         <f>G7/G8/4/3.14*10^7</f>
         <v>955.41401273885333</v>
       </c>
-      <c r="K19" s="14" t="s">
+      <c r="K19" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="L19" s="15" t="s">
+      <c r="L19" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="M19" s="15" t="s">
+      <c r="M19" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="20" spans="2:14">
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="9">
+      <c r="C20" s="7">
         <f>C15/C10</f>
         <v>6.666666666666667</v>
       </c>
-      <c r="D20" s="9">
+      <c r="D20" s="7">
         <f>C20/1000000</f>
         <v>6.6666666666666666E-6</v>
       </c>
-      <c r="K20" s="7" t="s">
+      <c r="K20" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="L20" s="7">
-        <v>0.106</v>
-      </c>
-      <c r="M20" s="7">
+      <c r="L20" s="5">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="M20" s="5">
         <f>L20*1000</f>
-        <v>106</v>
+        <v>176</v>
       </c>
       <c r="N20" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="21" spans="2:14">
-      <c r="G21" s="15" t="s">
+      <c r="G21" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="H21" s="15" t="s">
+      <c r="H21" s="13" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="22" spans="2:14">
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F22" s="9" t="s">
+      <c r="F22" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G22" s="10">
+      <c r="G22" s="8">
         <f>C6/4.44/L5/C8/G7</f>
         <v>0.37001287001287003</v>
       </c>
-      <c r="H22" s="9">
+      <c r="H22" s="7">
         <f>1000000*G22</f>
         <v>370012.87001287006</v>
       </c>
-      <c r="K22" s="9" t="s">
+      <c r="K22" s="7" t="s">
         <v>40</v>
       </c>
-      <c r="L22" s="9">
+      <c r="L22" s="7">
         <f>L14/L20</f>
-        <v>0.106340959499286</v>
-      </c>
-      <c r="M22" s="9">
+        <v>6.4046259698433611E-2</v>
+      </c>
+      <c r="M22" s="7">
         <f>M14/M20</f>
-        <v>106.340959499286</v>
+        <v>64.046259698433616</v>
       </c>
     </row>
     <row r="23" spans="2:14">
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="8">
+      <c r="C23" s="6">
         <v>1.24</v>
       </c>
-      <c r="D23" s="5">
+      <c r="D23" s="3">
         <f>SQRT(C19/3.14)</f>
         <v>1.2403664285993157</v>
       </c>
@@ -1255,297 +1255,297 @@
       </c>
     </row>
     <row r="24" spans="2:14" ht="15" customHeight="1">
-      <c r="B24" s="9" t="s">
+      <c r="B24" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="8">
+      <c r="C24" s="6">
         <v>1.4570000000000001</v>
       </c>
-      <c r="D24" s="5">
+      <c r="D24" s="3">
         <f>SQRT(C20/3.14)</f>
         <v>1.4571006315731201</v>
       </c>
-      <c r="G24" s="15" t="s">
+      <c r="G24" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H24" s="15" t="s">
+      <c r="H24" s="13" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="25" spans="2:14" ht="15" customHeight="1">
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="23" t="s">
         <v>68</v>
       </c>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="F25" s="9" t="s">
+      <c r="C25" s="23"/>
+      <c r="D25" s="23"/>
+      <c r="F25" s="7" t="s">
         <v>66</v>
       </c>
-      <c r="G25" s="9">
+      <c r="G25" s="7">
         <f>SQRT(G22)</f>
         <v>0.60828683202324052</v>
       </c>
-      <c r="H25" s="9">
+      <c r="H25" s="7">
         <f>SQRT(H22)</f>
         <v>608.28683202324055</v>
       </c>
-      <c r="I25" s="24" t="s">
+      <c r="I25" s="23" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="26" spans="2:14">
-      <c r="B26" s="24"/>
-      <c r="C26" s="24"/>
-      <c r="D26" s="24"/>
-      <c r="I26" s="24"/>
+      <c r="B26" s="23"/>
+      <c r="C26" s="23"/>
+      <c r="D26" s="23"/>
+      <c r="I26" s="23"/>
     </row>
     <row r="27" spans="2:14">
-      <c r="B27" s="24"/>
-      <c r="C27" s="24"/>
-      <c r="D27" s="24"/>
-      <c r="F27" s="14" t="s">
+      <c r="B27" s="23"/>
+      <c r="C27" s="23"/>
+      <c r="D27" s="23"/>
+      <c r="F27" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="G27" s="15" t="s">
+      <c r="G27" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H27" s="15" t="s">
+      <c r="H27" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I27" s="24"/>
+      <c r="I27" s="23"/>
     </row>
     <row r="28" spans="2:14">
-      <c r="F28" s="7" t="s">
+      <c r="F28" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="G28" s="7">
+      <c r="G28" s="5">
         <v>0.60799999999999998</v>
       </c>
-      <c r="H28" s="7">
+      <c r="H28" s="5">
         <f>G28*1000</f>
         <v>608</v>
       </c>
-      <c r="L28" s="15" t="s">
+      <c r="L28" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="29" spans="2:14">
-      <c r="K29" s="9" t="s">
+      <c r="K29" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="L29" s="9">
+      <c r="L29" s="7">
         <f>L20+2*G30</f>
-        <v>1.3231475987265462</v>
+        <v>1.393147598726546</v>
       </c>
     </row>
     <row r="30" spans="2:14">
-      <c r="C30" s="6" t="s">
+      <c r="C30" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="F30" s="9" t="s">
+      <c r="F30" s="7" t="s">
         <v>52</v>
       </c>
-      <c r="G30" s="9">
+      <c r="G30" s="7">
         <f>G22/G28</f>
         <v>0.60857379936327305</v>
       </c>
-      <c r="H30" s="9">
+      <c r="H30" s="7">
         <f>H22/H28</f>
         <v>608.57379936327311</v>
       </c>
-      <c r="K30" s="9" t="s">
+      <c r="K30" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="L30" s="9">
+      <c r="L30" s="7">
         <f>L22+2*G30</f>
-        <v>1.323488558225832</v>
+        <v>1.2811938584249798</v>
       </c>
     </row>
     <row r="31" spans="2:14">
-      <c r="B31" s="9" t="s">
+      <c r="B31" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="9">
+      <c r="C31" s="7">
         <f>SQRT(H28*H30)/2 + M22/4</f>
-        <v>330.7286558864418</v>
+        <v>320.1549809362287</v>
       </c>
       <c r="F31" t="s">
         <v>38</v>
       </c>
-      <c r="K31" s="22" t="s">
+      <c r="K31" s="21" t="s">
         <v>54</v>
       </c>
-      <c r="L31" s="22"/>
+      <c r="L31" s="21"/>
     </row>
     <row r="33" spans="2:12">
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D33" s="6" t="s">
+      <c r="D33" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="34" spans="2:12">
-      <c r="B34" s="9" t="s">
+      <c r="B34" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C34" s="9">
+      <c r="C34" s="7">
         <f>2*3.14*C31*L5</f>
-        <v>726941.58563839912</v>
-      </c>
-      <c r="D34" s="9">
+        <v>703700.64809783071</v>
+      </c>
+      <c r="D34" s="7">
         <f>C34/1000</f>
-        <v>726.94158563839915</v>
-      </c>
-      <c r="G34" s="16" t="s">
+        <v>703.70064809783071</v>
+      </c>
+      <c r="G34" s="14" t="s">
         <v>55</v>
       </c>
-      <c r="H34" s="16" t="s">
+      <c r="H34" s="14" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="35" spans="2:12">
-      <c r="B35" s="9" t="s">
+      <c r="B35" s="7" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="9">
+      <c r="C35" s="7">
         <f>2*3.14*C31*L6</f>
-        <v>526769.26495536172</v>
-      </c>
-      <c r="D35" s="9">
+        <v>509928.00586799328</v>
+      </c>
+      <c r="D35" s="7">
         <f>C35/1000</f>
-        <v>526.76926495536168</v>
-      </c>
-      <c r="F35" s="9" t="s">
+        <v>509.92800586799331</v>
+      </c>
+      <c r="F35" s="7" t="s">
         <v>50</v>
       </c>
-      <c r="G35" s="9">
+      <c r="G35" s="7">
         <f>(L29*L30-L20*L22)*G28*1000000*G10</f>
-        <v>8304187.8760512844</v>
-      </c>
-      <c r="H35" s="9">
+        <v>8465133.5630189832</v>
+      </c>
+      <c r="H35" s="7">
         <f>G35/1000</f>
-        <v>8304.1878760512845</v>
-      </c>
-      <c r="L35" s="15" t="s">
+        <v>8465.1335630189824</v>
+      </c>
+      <c r="L35" s="13" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="36" spans="2:12">
-      <c r="K36" s="9" t="s">
+      <c r="K36" s="7" t="s">
         <v>65</v>
       </c>
-      <c r="L36" s="9">
+      <c r="L36" s="7">
         <f>2*L20+2*L22+4*G30</f>
-        <v>2.8589771164516642</v>
+        <v>2.9143877168499595</v>
       </c>
     </row>
     <row r="39" spans="2:12">
-      <c r="B39" s="9" t="s">
+      <c r="B39" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="C39" s="9">
+      <c r="C39" s="7">
         <f>G14*D34/D19</f>
-        <v>2.5280120582160972</v>
+        <v>2.4471893738250161</v>
       </c>
     </row>
     <row r="40" spans="2:12">
-      <c r="B40" s="9" t="s">
+      <c r="B40" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="C40" s="9">
+      <c r="C40" s="7">
         <f>G14*D35/3.14/(C24*0.001)^2</f>
-        <v>1.3276419229175465</v>
-      </c>
-      <c r="K40" s="9" t="s">
+        <v>1.2851960873561246</v>
+      </c>
+      <c r="K40" s="7" t="s">
         <v>70</v>
       </c>
-      <c r="L40" s="9">
+      <c r="L40" s="7">
         <f>L36/G22/G18</f>
-        <v>6438.9136796607045</v>
+        <v>6563.7079883838223</v>
       </c>
     </row>
     <row r="42" spans="2:12">
-      <c r="B42" s="19" t="s">
+      <c r="B42" s="17" t="s">
         <v>46</v>
       </c>
-      <c r="C42" s="20">
+      <c r="C42" s="18">
         <f>(C14^2)*C39</f>
-        <v>530.98341907500469</v>
-      </c>
-      <c r="K42" s="9" t="s">
+        <v>514.00742991493723</v>
+      </c>
+      <c r="K42" s="7" t="s">
         <v>71</v>
       </c>
-      <c r="L42" s="9">
+      <c r="L42" s="7">
         <f>(L5^2)/L40</f>
-        <v>19.024948321166978</v>
+        <v>18.663231243192936</v>
       </c>
     </row>
     <row r="43" spans="2:12">
-      <c r="B43" s="19" t="s">
+      <c r="B43" s="17" t="s">
         <v>47</v>
       </c>
-      <c r="C43" s="20">
+      <c r="C43" s="18">
         <f>(C15^2)*C40</f>
-        <v>531.05676916701862</v>
-      </c>
-      <c r="K43" s="9" t="s">
+        <v>514.0784349424498</v>
+      </c>
+      <c r="K43" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="L43" s="9">
+      <c r="L43" s="7">
         <f>L6^2/L40</f>
-        <v>9.9899959678465553</v>
+        <v>9.8000584137749094</v>
       </c>
     </row>
     <row r="44" spans="2:12">
-      <c r="B44" s="19" t="s">
+      <c r="B44" s="17" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="20">
+      <c r="C44" s="18">
         <f>C42+C43</f>
-        <v>1062.0401882420233</v>
-      </c>
-      <c r="F44" s="19" t="s">
+        <v>1028.0858648573872</v>
+      </c>
+      <c r="F44" s="17" t="s">
         <v>57</v>
       </c>
-      <c r="G44" s="19">
+      <c r="G44" s="17">
         <f>G9*(G7^2)*H35</f>
-        <v>11360.129014438156</v>
+        <v>11580.302714209967</v>
       </c>
     </row>
     <row r="48" spans="2:12">
-      <c r="D48" s="4" t="s">
+      <c r="D48" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="E48" s="4">
+      <c r="E48" s="2">
         <f>C5*C12/(C5*C12+C42+C43+G44)</f>
-        <v>0.9757579395481486</v>
+        <v>0.97540346810551148</v>
       </c>
     </row>
     <row r="51" spans="8:10">
-      <c r="H51" s="2" t="s">
+      <c r="H51" s="24" t="s">
         <v>73</v>
       </c>
-      <c r="I51" s="2"/>
-      <c r="J51" s="2"/>
+      <c r="I51" s="24"/>
+      <c r="J51" s="24"/>
     </row>
     <row r="52" spans="8:10">
-      <c r="H52" s="2"/>
-      <c r="I52" s="2"/>
-      <c r="J52" s="2"/>
+      <c r="H52" s="24"/>
+      <c r="I52" s="24"/>
+      <c r="J52" s="24"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="F12:G12"/>
+    <mergeCell ref="B25:D27"/>
     <mergeCell ref="K31:L31"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="N16:N18"/>
     <mergeCell ref="H51:J52"/>
     <mergeCell ref="I25:I27"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="F12:G12"/>
-    <mergeCell ref="B25:D27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Q1 partA, Q2 tamamlandı
</commit_message>
<xml_diff>
--- a/Project1/p1_question2.xlsx
+++ b/Project1/p1_question2.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="85">
   <si>
     <t>Iin</t>
   </si>
@@ -180,9 +180,6 @@
     <t>A</t>
   </si>
   <si>
-    <t>aşagıdaki figür referans alınmıştır</t>
-  </si>
-  <si>
     <t>g</t>
   </si>
   <si>
@@ -201,9 +198,6 @@
     <t>Total Copper loss(W)</t>
   </si>
   <si>
-    <t>B-H curve kullanılarak yazılır</t>
-  </si>
-  <si>
     <t>*Bop^2, laminasyona göre değişir</t>
   </si>
   <si>
@@ -219,9 +213,6 @@
     <t>x1(D),x2(E,R)</t>
   </si>
   <si>
-    <t>!! Kare ise aşağıdaki inputa bu değer yazılır</t>
-  </si>
-  <si>
     <t>copper yarıcapları akım density sabit alınarak heaplanmıştır,duruma göre ayarlanabilir, sağdaki densityden hesaplanan değer inputa yazılır</t>
   </si>
   <si>
@@ -237,9 +228,6 @@
     <t>squere-core</t>
   </si>
   <si>
-    <t>aşağıda görsel boyutları göstermek içindir.</t>
-  </si>
-  <si>
     <t>lamination type</t>
   </si>
   <si>
@@ -249,16 +237,49 @@
     <t>material cost ($/kg)</t>
   </si>
   <si>
-    <t>cable cost($/m)</t>
-  </si>
-  <si>
     <t>outer inductance,L2(H)</t>
+  </si>
+  <si>
+    <t>mutual inductance(H)</t>
+  </si>
+  <si>
+    <t>core cost</t>
+  </si>
+  <si>
+    <t>cable cost in($/m)</t>
+  </si>
+  <si>
+    <t>cable cost out($/m)</t>
+  </si>
+  <si>
+    <t>inner cable cost</t>
+  </si>
+  <si>
+    <t>outer cable cost</t>
+  </si>
+  <si>
+    <t>Total cost</t>
+  </si>
+  <si>
+    <t xml:space="preserve">write by using B-H curve </t>
+  </si>
+  <si>
+    <t>!! İf it is square this value can be write input at left</t>
+  </si>
+  <si>
+    <t>next figure is using only figure dimensions.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">taking reference from dimension figure </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="[$$-409]#,##0"/>
+  </numFmts>
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -294,7 +315,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="13">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -356,6 +377,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC00000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -433,12 +460,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -460,12 +486,6 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="2" xfId="2" applyFill="1"/>
     <xf numFmtId="2" fontId="2" fillId="11" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -478,6 +498,16 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="11" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="2" applyFill="1"/>
+    <xf numFmtId="166" fontId="2" fillId="7" borderId="2" xfId="2" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Çıkış" xfId="2" builtinId="21"/>
@@ -494,15 +524,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>1</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>161925</xdr:rowOff>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>59</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>78</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -520,7 +550,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="1133475" y="10067925"/>
+          <a:off x="1076325" y="11496675"/>
           <a:ext cx="4819650" cy="3505200"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -541,15 +571,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>1000125</xdr:colOff>
-      <xdr:row>52</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:colOff>1009650</xdr:colOff>
+      <xdr:row>57</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>1143000</xdr:colOff>
-      <xdr:row>71</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:colOff>1152525</xdr:colOff>
+      <xdr:row>75</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -567,7 +597,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="6924675" y="9982200"/>
+          <a:off x="8039100" y="11001375"/>
           <a:ext cx="5362575" cy="3562350"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -873,10 +903,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B1:N52"/>
+  <dimension ref="B1:N57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="L6" sqref="L6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F55" sqref="F55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -896,357 +926,367 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:14">
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="3" spans="2:14">
-      <c r="F3" s="25" t="s">
+      <c r="F3" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="25"/>
+      <c r="G3" s="22"/>
     </row>
     <row r="4" spans="2:14">
-      <c r="B4" s="25" t="s">
+      <c r="B4" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="F4" s="5" t="s">
+      <c r="C4" s="22"/>
+      <c r="F4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="K4" s="25" t="s">
+      <c r="G4" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K4" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="L4" s="25"/>
+      <c r="L4" s="22"/>
     </row>
     <row r="5" spans="2:14">
-      <c r="B5" s="5" t="s">
+      <c r="B5" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="15">
+      <c r="C5" s="14">
         <v>500000</v>
       </c>
-      <c r="F5" s="5" t="s">
-        <v>74</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>75</v>
-      </c>
-      <c r="K5" s="5" t="s">
+      <c r="F5" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>71</v>
+      </c>
+      <c r="K5" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="L5" s="11">
-        <v>350</v>
+      <c r="L5" s="10">
+        <v>1200</v>
       </c>
     </row>
     <row r="6" spans="2:14">
-      <c r="B6" s="5" t="s">
+      <c r="B6" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="14">
         <v>34500</v>
       </c>
-      <c r="F6" s="5" t="s">
+      <c r="F6" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="5" t="s">
+      <c r="G6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="K6" s="7" t="s">
+      <c r="K6" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="L6" s="10">
+      <c r="L6" s="9">
         <f>L5/L9</f>
-        <v>253.62318840579712</v>
+        <v>869.56521739130437</v>
       </c>
     </row>
     <row r="7" spans="2:14">
-      <c r="B7" s="5" t="s">
+      <c r="B7" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C7" s="15">
+      <c r="C7" s="14">
         <v>25000</v>
       </c>
-      <c r="F7" s="5" t="s">
+      <c r="F7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G7" s="15">
+      <c r="G7" s="14">
         <v>1.2</v>
       </c>
-      <c r="H7" s="22" t="s">
-        <v>61</v>
+      <c r="H7" s="19" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="2:14">
-      <c r="B8" s="5" t="s">
+      <c r="B8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="15">
+      <c r="C8" s="14">
         <v>50</v>
       </c>
-      <c r="F8" s="5" t="s">
+      <c r="F8" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="15">
+      <c r="G8" s="14">
         <v>1000</v>
       </c>
-      <c r="H8" s="22"/>
+      <c r="H8" s="19"/>
     </row>
     <row r="9" spans="2:14" ht="24.75">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="C9" s="15">
+      <c r="C9" s="14">
         <v>40</v>
       </c>
-      <c r="F9" s="5" t="s">
+      <c r="F9" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="G9" s="15">
+      <c r="G9" s="14">
         <v>0.95</v>
       </c>
-      <c r="H9" s="20" t="s">
-        <v>62</v>
-      </c>
-      <c r="K9" s="7" t="s">
+      <c r="H9" s="25" t="s">
+        <v>60</v>
+      </c>
+      <c r="K9" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="L9" s="8">
+      <c r="L9" s="7">
         <f>C6/C7</f>
         <v>1.38</v>
       </c>
     </row>
     <row r="10" spans="2:14">
-      <c r="B10" s="5" t="s">
+      <c r="B10" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="15">
+      <c r="C10" s="14">
         <v>3</v>
       </c>
-      <c r="F10" s="9" t="s">
+      <c r="F10" s="8" t="s">
         <v>51</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="18">
         <v>7.85</v>
       </c>
     </row>
     <row r="11" spans="2:14">
-      <c r="B11" s="5" t="s">
+      <c r="B11" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="14">
         <v>0.3</v>
       </c>
-      <c r="F11" s="5" t="s">
-        <v>76</v>
-      </c>
-      <c r="G11" s="5"/>
+      <c r="F11" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="G11" s="4">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" spans="2:14">
-      <c r="B12" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="C12" s="15">
+      <c r="B12" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="C12" s="14">
         <v>1</v>
       </c>
-      <c r="F12" s="25" t="s">
+      <c r="F12" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="G12" s="25"/>
+      <c r="G12" s="22"/>
     </row>
     <row r="13" spans="2:14">
-      <c r="F13" s="5" t="s">
+      <c r="F13" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="G13" s="5" t="s">
+      <c r="G13" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="L13" s="14" t="s">
+      <c r="L13" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="M13" s="14" t="s">
+      <c r="M13" s="13" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="2:14">
-      <c r="B14" s="7" t="s">
+      <c r="B14" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C14" s="8">
+      <c r="C14" s="7">
         <f>C5/C6</f>
         <v>14.492753623188406</v>
       </c>
-      <c r="F14" s="5" t="s">
+      <c r="F14" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="G14" s="15">
+      <c r="G14" s="14">
         <v>1.6800000000000002E-8</v>
       </c>
-      <c r="K14" s="7" t="s">
+      <c r="K14" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="L14" s="7">
+      <c r="L14" s="6">
         <f>M14/10^6</f>
-        <v>1.1272141706924315E-2</v>
-      </c>
-      <c r="M14" s="7">
+        <v>3.8647342995169087E-2</v>
+      </c>
+      <c r="M14" s="6">
         <f>(L5*C19+L6*C20)/C11</f>
-        <v>11272.141706924316</v>
+        <v>38647.342995169085</v>
       </c>
     </row>
     <row r="15" spans="2:14">
-      <c r="B15" s="7" t="s">
+      <c r="B15" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="8">
+      <c r="C15" s="7">
         <f>C5/C7</f>
         <v>20</v>
       </c>
-      <c r="F15" s="5" t="s">
+      <c r="F15" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="2:14">
+      <c r="F16" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="G15" s="5"/>
-    </row>
-    <row r="16" spans="2:14">
-      <c r="K16" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="L16" s="7">
+      <c r="G16" s="4">
+        <v>1</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="L16" s="6">
         <f>SQRT(L14)</f>
-        <v>0.10617034287843435</v>
-      </c>
-      <c r="M16" s="7">
+        <v>0.19658927487319619</v>
+      </c>
+      <c r="M16" s="6">
         <f>SQRT(M14)</f>
-        <v>106.17034287843435</v>
-      </c>
-      <c r="N16" s="23" t="s">
-        <v>67</v>
+        <v>196.58927487319619</v>
+      </c>
+      <c r="N16" s="20" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="2:14">
       <c r="H17" s="1"/>
-      <c r="N17" s="23"/>
+      <c r="N17" s="20"/>
     </row>
     <row r="18" spans="2:14">
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="D18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F18" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="G18" s="16">
+      <c r="F18" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="G18" s="15">
         <f>G7/G8</f>
         <v>1.1999999999999999E-3</v>
       </c>
-      <c r="N18" s="23"/>
+      <c r="N18" s="20"/>
     </row>
     <row r="19" spans="2:14">
-      <c r="B19" s="7" t="s">
+      <c r="B19" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="6">
         <f>C14/C10</f>
         <v>4.8309178743961354</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="6">
         <f>C19/1000000</f>
         <v>4.8309178743961353E-6</v>
       </c>
-      <c r="F19" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="G19" s="16">
+      <c r="F19" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="G19" s="15">
         <f>G7/G8/4/3.14*10^7</f>
         <v>955.41401273885333</v>
       </c>
-      <c r="K19" s="12" t="s">
+      <c r="K19" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="L19" s="13" t="s">
+      <c r="L19" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="M19" s="13" t="s">
+      <c r="M19" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="20" spans="2:14">
-      <c r="B20" s="7" t="s">
+      <c r="B20" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="6">
         <f>C15/C10</f>
         <v>6.666666666666667</v>
       </c>
-      <c r="D20" s="7">
+      <c r="D20" s="6">
         <f>C20/1000000</f>
         <v>6.6666666666666666E-6</v>
       </c>
-      <c r="K20" s="5" t="s">
+      <c r="K20" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="L20" s="5">
-        <v>0.17599999999999999</v>
-      </c>
-      <c r="M20" s="5">
+      <c r="L20" s="4">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="M20" s="4">
         <f>L20*1000</f>
-        <v>176</v>
+        <v>196</v>
       </c>
       <c r="N20" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="21" spans="2:14">
-      <c r="G21" s="13" t="s">
+      <c r="G21" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="H21" s="13" t="s">
+      <c r="H21" s="12" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="22" spans="2:14">
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F22" s="7" t="s">
+      <c r="F22" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="G22" s="8">
+      <c r="G22" s="7">
         <f>C6/4.44/L5/C8/G7</f>
-        <v>0.37001287001287003</v>
-      </c>
-      <c r="H22" s="7">
+        <v>0.10792042042042044</v>
+      </c>
+      <c r="H22" s="6">
         <f>1000000*G22</f>
-        <v>370012.87001287006</v>
-      </c>
-      <c r="K22" s="7" t="s">
+        <v>107920.42042042044</v>
+      </c>
+      <c r="K22" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="L22" s="7">
+      <c r="L22" s="6">
         <f>L14/L20</f>
-        <v>6.4046259698433611E-2</v>
-      </c>
-      <c r="M22" s="7">
+        <v>0.19718032140392391</v>
+      </c>
+      <c r="M22" s="6">
         <f>M14/M20</f>
-        <v>64.046259698433616</v>
+        <v>197.1803214039239</v>
       </c>
     </row>
     <row r="23" spans="2:14">
-      <c r="B23" s="7" t="s">
+      <c r="B23" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C23" s="6">
+      <c r="C23" s="5">
         <v>1.24</v>
       </c>
-      <c r="D23" s="3">
+      <c r="D23" s="2">
         <f>SQRT(C19/3.14)</f>
         <v>1.2403664285993157</v>
       </c>
@@ -1255,287 +1295,341 @@
       </c>
     </row>
     <row r="24" spans="2:14" ht="15" customHeight="1">
-      <c r="B24" s="7" t="s">
+      <c r="B24" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="6">
+      <c r="C24" s="5">
         <v>1.4570000000000001</v>
       </c>
-      <c r="D24" s="3">
+      <c r="D24" s="2">
         <f>SQRT(C20/3.14)</f>
         <v>1.4571006315731201</v>
       </c>
-      <c r="G24" s="13" t="s">
+      <c r="G24" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="H24" s="13" t="s">
+      <c r="H24" s="12" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="25" spans="2:14" ht="15" customHeight="1">
-      <c r="B25" s="23" t="s">
-        <v>68</v>
-      </c>
-      <c r="C25" s="23"/>
-      <c r="D25" s="23"/>
-      <c r="F25" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="G25" s="7">
+      <c r="B25" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C25" s="20"/>
+      <c r="D25" s="20"/>
+      <c r="F25" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="G25" s="6">
         <f>SQRT(G22)</f>
-        <v>0.60828683202324052</v>
-      </c>
-      <c r="H25" s="7">
+        <v>0.32851243571655009</v>
+      </c>
+      <c r="H25" s="6">
         <f>SQRT(H22)</f>
-        <v>608.28683202324055</v>
-      </c>
-      <c r="I25" s="23" t="s">
-        <v>67</v>
+        <v>328.51243571655004</v>
+      </c>
+      <c r="I25" s="20" t="s">
+        <v>82</v>
       </c>
     </row>
     <row r="26" spans="2:14">
-      <c r="B26" s="23"/>
-      <c r="C26" s="23"/>
-      <c r="D26" s="23"/>
-      <c r="I26" s="23"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="20"/>
+      <c r="D26" s="20"/>
+      <c r="I26" s="20"/>
     </row>
     <row r="27" spans="2:14">
-      <c r="B27" s="23"/>
-      <c r="C27" s="23"/>
-      <c r="D27" s="23"/>
-      <c r="F27" s="12" t="s">
+      <c r="B27" s="20"/>
+      <c r="C27" s="20"/>
+      <c r="D27" s="20"/>
+      <c r="F27" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="G27" s="13" t="s">
+      <c r="G27" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="H27" s="13" t="s">
+      <c r="H27" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="I27" s="23"/>
+      <c r="I27" s="20"/>
     </row>
     <row r="28" spans="2:14">
-      <c r="F28" s="5" t="s">
+      <c r="F28" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="G28" s="5">
-        <v>0.60799999999999998</v>
-      </c>
-      <c r="H28" s="5">
+      <c r="G28" s="4">
+        <v>0.36</v>
+      </c>
+      <c r="H28" s="4">
         <f>G28*1000</f>
-        <v>608</v>
-      </c>
-      <c r="L28" s="13" t="s">
+        <v>360</v>
+      </c>
+      <c r="L28" s="12" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="29" spans="2:14">
-      <c r="K29" s="7" t="s">
+      <c r="K29" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="L29" s="7">
+      <c r="L29" s="6">
         <f>L20+2*G30</f>
-        <v>1.393147598726546</v>
+        <v>0.795557891224558</v>
       </c>
     </row>
     <row r="30" spans="2:14">
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F30" s="7" t="s">
+      <c r="F30" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="G30" s="7">
+      <c r="G30" s="6">
         <f>G22/G28</f>
-        <v>0.60857379936327305</v>
-      </c>
-      <c r="H30" s="7">
+        <v>0.29977894561227902</v>
+      </c>
+      <c r="H30" s="6">
         <f>H22/H28</f>
-        <v>608.57379936327311</v>
-      </c>
-      <c r="K30" s="7" t="s">
+        <v>299.77894561227902</v>
+      </c>
+      <c r="K30" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="L30" s="7">
+      <c r="L30" s="6">
         <f>L22+2*G30</f>
-        <v>1.2811938584249798</v>
+        <v>0.79673821262848199</v>
       </c>
     </row>
     <row r="31" spans="2:14">
-      <c r="B31" s="7" t="s">
+      <c r="B31" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C31" s="7">
+      <c r="C31" s="6">
         <f>SQRT(H28*H30)/2 + M22/4</f>
-        <v>320.1549809362287</v>
+        <v>213.551298209256</v>
       </c>
       <c r="F31" t="s">
         <v>38</v>
       </c>
-      <c r="K31" s="21" t="s">
+      <c r="K31" s="24" t="s">
+        <v>84</v>
+      </c>
+      <c r="L31" s="24"/>
+    </row>
+    <row r="33" spans="2:12">
+      <c r="C33" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" s="3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="2:12">
+      <c r="B34" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C34" s="6">
+        <f>2*3.14*C31*L5</f>
+        <v>1609322.5833049533</v>
+      </c>
+      <c r="D34" s="6">
+        <f>C34/1000</f>
+        <v>1609.3225833049532</v>
+      </c>
+      <c r="G34" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="L31" s="21"/>
-    </row>
-    <row r="33" spans="2:12">
-      <c r="C33" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="D33" s="4" t="s">
+      <c r="H34" s="13" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="35" spans="2:12">
+      <c r="B35" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C35" s="6">
+        <f>2*3.14*C31*L6</f>
+        <v>1166175.7850035892</v>
+      </c>
+      <c r="D35" s="6">
+        <f>C35/1000</f>
+        <v>1166.1757850035892</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G35" s="6">
+        <f>(L29*L30-L20*L22)*G28*1000000*G10</f>
+        <v>1682046.5868062354</v>
+      </c>
+      <c r="H35" s="6">
+        <f>G35/1000</f>
+        <v>1682.0465868062354</v>
+      </c>
+      <c r="L35" s="12" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="34" spans="2:12">
-      <c r="B34" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" s="7">
-        <f>2*3.14*C31*L5</f>
-        <v>703700.64809783071</v>
-      </c>
-      <c r="D34" s="7">
-        <f>C34/1000</f>
-        <v>703.70064809783071</v>
-      </c>
-      <c r="G34" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="H34" s="14" t="s">
+    <row r="36" spans="2:12">
+      <c r="K36" s="6" t="s">
+        <v>63</v>
+      </c>
+      <c r="L36" s="6">
+        <f>2*L20+2*L22+4*G30</f>
+        <v>1.9854764252569639</v>
+      </c>
+    </row>
+    <row r="39" spans="2:12">
+      <c r="B39" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C39" s="6">
+        <f>G14*D34/D19</f>
+        <v>5.596580215701306</v>
+      </c>
+    </row>
+    <row r="40" spans="2:12">
+      <c r="B40" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="C40" s="6">
+        <f>G14*D35/3.14/(C24*0.001)^2</f>
+        <v>2.9391689391620903</v>
+      </c>
+      <c r="K40" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="L40" s="6">
+        <f>L36/G22/G18</f>
+        <v>15331.331005462467</v>
+      </c>
+    </row>
+    <row r="42" spans="2:12">
+      <c r="B42" s="16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C42" s="17">
+        <f>(C14^2)*C39</f>
+        <v>1175.5051912836182</v>
+      </c>
+    </row>
+    <row r="43" spans="2:12">
+      <c r="B43" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="C43" s="17">
+        <f>(C15^2)*C40</f>
+        <v>1175.667575664836</v>
+      </c>
+    </row>
+    <row r="44" spans="2:12">
+      <c r="B44" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="C44" s="17">
+        <f>C42+C43</f>
+        <v>2351.1727669484544</v>
+      </c>
+      <c r="F44" s="16" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="35" spans="2:12">
-      <c r="B35" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C35" s="7">
-        <f>2*3.14*C31*L6</f>
-        <v>509928.00586799328</v>
-      </c>
-      <c r="D35" s="7">
-        <f>C35/1000</f>
-        <v>509.92800586799331</v>
-      </c>
-      <c r="F35" s="7" t="s">
-        <v>50</v>
-      </c>
-      <c r="G35" s="7">
-        <f>(L29*L30-L20*L22)*G28*1000000*G10</f>
-        <v>8465133.5630189832</v>
-      </c>
-      <c r="H35" s="7">
-        <f>G35/1000</f>
-        <v>8465.1335630189824</v>
-      </c>
-      <c r="L35" s="13" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="36" spans="2:12">
-      <c r="K36" s="7" t="s">
-        <v>65</v>
-      </c>
-      <c r="L36" s="7">
-        <f>2*L20+2*L22+4*G30</f>
-        <v>2.9143877168499595</v>
-      </c>
-    </row>
-    <row r="39" spans="2:12">
-      <c r="B39" s="7" t="s">
-        <v>48</v>
-      </c>
-      <c r="C39" s="7">
-        <f>G14*D34/D19</f>
-        <v>2.4471893738250161</v>
-      </c>
-    </row>
-    <row r="40" spans="2:12">
-      <c r="B40" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="C40" s="7">
-        <f>G14*D35/3.14/(C24*0.001)^2</f>
-        <v>1.2851960873561246</v>
-      </c>
-      <c r="K40" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="L40" s="7">
-        <f>L36/G22/G18</f>
-        <v>6563.7079883838223</v>
-      </c>
-    </row>
-    <row r="42" spans="2:12">
-      <c r="B42" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C42" s="18">
-        <f>(C14^2)*C39</f>
-        <v>514.00742991493723</v>
-      </c>
-      <c r="K42" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="L42" s="7">
+      <c r="G44" s="16">
+        <f>G9*(G7^2)*H35</f>
+        <v>2301.0397307509297</v>
+      </c>
+    </row>
+    <row r="45" spans="2:12">
+      <c r="K45" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="L45" s="16">
         <f>(L5^2)/L40</f>
-        <v>18.663231243192936</v>
-      </c>
-    </row>
-    <row r="43" spans="2:12">
-      <c r="B43" s="17" t="s">
-        <v>47</v>
-      </c>
-      <c r="C43" s="18">
-        <f>(C15^2)*C40</f>
-        <v>514.0784349424498</v>
-      </c>
-      <c r="K43" s="7" t="s">
+        <v>93.925308865025229</v>
+      </c>
+    </row>
+    <row r="46" spans="2:12">
+      <c r="K46" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="L46" s="16">
+        <f>L6^2/L40</f>
+        <v>49.320157984155237</v>
+      </c>
+    </row>
+    <row r="47" spans="2:12">
+      <c r="K47" s="16" t="s">
+        <v>74</v>
+      </c>
+      <c r="L47" s="16">
+        <f>L5/L40*L6</f>
+        <v>68.061818018134218</v>
+      </c>
+    </row>
+    <row r="48" spans="2:12">
+      <c r="D48" s="27" t="s">
+        <v>57</v>
+      </c>
+      <c r="E48" s="27">
+        <f>C5*C12/(C5*C12+C42+C43+G44)</f>
+        <v>0.99078134924907202</v>
+      </c>
+      <c r="G48" s="16" t="s">
+        <v>75</v>
+      </c>
+      <c r="H48" s="26">
+        <f>H35*G11</f>
+        <v>5046.1397604187059</v>
+      </c>
+    </row>
+    <row r="49" spans="7:10">
+      <c r="G49" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="L43" s="7">
-        <f>L6^2/L40</f>
-        <v>9.8000584137749094</v>
-      </c>
-    </row>
-    <row r="44" spans="2:12">
-      <c r="B44" s="17" t="s">
-        <v>60</v>
-      </c>
-      <c r="C44" s="18">
-        <f>C42+C43</f>
-        <v>1028.0858648573872</v>
-      </c>
-      <c r="F44" s="17" t="s">
-        <v>57</v>
-      </c>
-      <c r="G44" s="17">
-        <f>G9*(G7^2)*H35</f>
-        <v>11580.302714209967</v>
-      </c>
-    </row>
-    <row r="48" spans="2:12">
-      <c r="D48" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="E48" s="2">
-        <f>C5*C12/(C5*C12+C42+C43+G44)</f>
-        <v>0.97540346810551148</v>
-      </c>
-    </row>
-    <row r="51" spans="8:10">
-      <c r="H51" s="24" t="s">
-        <v>73</v>
-      </c>
-      <c r="I51" s="24"/>
-      <c r="J51" s="24"/>
-    </row>
-    <row r="52" spans="8:10">
-      <c r="H52" s="24"/>
-      <c r="I52" s="24"/>
-      <c r="J52" s="24"/>
+      <c r="H49" s="26">
+        <f>D34*G15</f>
+        <v>1609.3225833049532</v>
+      </c>
+    </row>
+    <row r="50" spans="7:10">
+      <c r="G50" s="16" t="s">
+        <v>79</v>
+      </c>
+      <c r="H50" s="26">
+        <f>D35*G16</f>
+        <v>1166.1757850035892</v>
+      </c>
+    </row>
+    <row r="51" spans="7:10">
+      <c r="G51" s="27" t="s">
+        <v>80</v>
+      </c>
+      <c r="H51" s="28">
+        <f>H48+H49+H50</f>
+        <v>7821.6381287272479</v>
+      </c>
+      <c r="I51" s="23"/>
+      <c r="J51" s="23"/>
+    </row>
+    <row r="52" spans="7:10">
+      <c r="I52" s="23"/>
+      <c r="J52" s="23"/>
+    </row>
+    <row r="56" spans="7:10">
+      <c r="H56" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="I56" s="21"/>
+      <c r="J56" s="21"/>
+    </row>
+    <row r="57" spans="7:10">
+      <c r="H57" s="21"/>
+      <c r="I57" s="21"/>
+      <c r="J57" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="H56:J57"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="K4:L4"/>
@@ -1544,7 +1638,6 @@
     <mergeCell ref="K31:L31"/>
     <mergeCell ref="H7:H8"/>
     <mergeCell ref="N16:N18"/>
-    <mergeCell ref="H51:J52"/>
     <mergeCell ref="I25:I27"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>